<commit_message>
Update all column name.
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_Ver1.1_ANH_THANG_LE.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_Ver1.1_ANH_THANG_LE.xlsx
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="237">
   <si>
     <t>No</t>
   </si>
@@ -504,9 +504,6 @@
     <t xml:space="preserve">description </t>
   </si>
   <si>
-    <t>id_author</t>
-  </si>
-  <si>
     <t>avatar</t>
   </si>
   <si>
@@ -528,12 +525,6 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>id_user</t>
-  </si>
-  <si>
-    <t>id_post</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -700,9 +691,6 @@
   </si>
   <si>
     <t>Post Info</t>
-  </si>
-  <si>
-    <t>id_category</t>
   </si>
   <si>
     <t>Id category</t>
@@ -813,6 +801,21 @@
   </si>
   <si>
     <t>le.thang@moludo.com</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post_id </t>
+  </si>
+  <si>
+    <t>post_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_id </t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -8105,13 +8108,13 @@
     <row r="4" spans="2:6">
       <c r="B4" s="97"/>
       <c r="C4" s="114" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D4" s="94" t="s">
         <v>126</v>
       </c>
       <c r="E4" s="99" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F4" s="100"/>
     </row>
@@ -8405,7 +8408,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8414,10 +8417,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8426,7 +8429,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="123" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C7" s="124"/>
     </row>
@@ -8627,8 +8630,8 @@
   </sheetPr>
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q15" sqref="I12:U15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -8696,7 +8699,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="224" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G4" s="225"/>
     </row>
@@ -8736,7 +8739,7 @@
     </row>
     <row r="8" spans="1:21" ht="12" customHeight="1">
       <c r="B8" s="211" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C8" s="212"/>
       <c r="D8" s="212"/>
@@ -8800,25 +8803,25 @@
         <v>116</v>
       </c>
       <c r="L13" s="187" t="s">
+        <v>138</v>
+      </c>
+      <c r="M13" s="187" t="s">
         <v>139</v>
       </c>
-      <c r="M13" s="187" t="s">
-        <v>140</v>
-      </c>
       <c r="N13" s="187" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O13" s="187" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P13" s="187" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q13" s="187" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R13" s="194" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="S13" s="194" t="s">
         <v>128</v>
@@ -8841,7 +8844,7 @@
         <v>114</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -8861,22 +8864,22 @@
         <v>111</v>
       </c>
       <c r="L14" s="186" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="M14" s="186" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="N14" s="186">
         <v>0</v>
       </c>
       <c r="O14" s="186" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="P14" s="191" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="Q14" s="191" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="R14" s="186">
         <v>11000</v>
@@ -8897,7 +8900,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C15" s="65" t="s">
         <v>107</v>
@@ -8910,7 +8913,7 @@
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="186">
@@ -8923,22 +8926,22 @@
         <v>113</v>
       </c>
       <c r="L15" s="186" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="M15" s="186" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="N15" s="186">
         <v>1</v>
       </c>
       <c r="O15" s="186" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="P15" s="191" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="Q15" s="191" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="R15" s="186">
         <v>11000</v>
@@ -8959,7 +8962,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C16" s="65" t="s">
         <v>116</v>
@@ -8972,7 +8975,7 @@
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -8982,20 +8985,20 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -9004,20 +9007,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="117" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -9026,20 +9029,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -9048,10 +9051,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D20" s="129" t="s">
         <v>118</v>
@@ -9063,7 +9066,7 @@
         <v>99</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -9072,22 +9075,22 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="129" t="s">
         <v>178</v>
       </c>
-      <c r="C21" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" s="129" t="s">
-        <v>181</v>
-      </c>
       <c r="E21" s="66" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F21" s="67" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G21" s="106" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15">
@@ -9096,20 +9099,20 @@
         <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E22" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="67"/>
       <c r="G22" s="106" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H22" s="136"/>
     </row>
@@ -9119,20 +9122,20 @@
         <v>10</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" s="129" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E23" s="66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F23" s="67"/>
       <c r="G23" s="106" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -9141,20 +9144,20 @@
         <v>11</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E24" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="67"/>
       <c r="G24" s="106" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -9169,14 +9172,14 @@
         <v>128</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E25" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="67"/>
       <c r="G25" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -9191,14 +9194,14 @@
         <v>129</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E26" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="67"/>
       <c r="G26" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="12.75" thickBot="1">
@@ -9216,7 +9219,7 @@
         <v>118</v>
       </c>
       <c r="E27" s="155" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F27" s="158" t="s">
         <v>99</v>
@@ -9278,20 +9281,20 @@
         <v>2</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C32" s="204" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D32" s="205"/>
       <c r="E32" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="G32" s="53" t="s">
         <v>151</v>
-      </c>
-      <c r="F32" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="53" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
@@ -9401,8 +9404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -9471,7 +9474,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="224" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G4" s="225"/>
     </row>
@@ -9480,7 +9483,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="224" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D5" s="227"/>
       <c r="E5" s="42"/>
@@ -9511,7 +9514,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="B8" s="228" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C8" s="212"/>
       <c r="D8" s="212"/>
@@ -9580,7 +9583,7 @@
         <v>114</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -9590,7 +9593,7 @@
         <v>50</v>
       </c>
       <c r="I14" s="186" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J14" s="187" t="s">
         <v>127</v>
@@ -9605,7 +9608,7 @@
         <v>132</v>
       </c>
       <c r="N14" s="187" t="s">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="O14" s="186" t="s">
         <v>128</v>
@@ -9629,7 +9632,7 @@
         <v>127</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -9642,25 +9645,25 @@
         <v>1</v>
       </c>
       <c r="J15" s="190" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="K15" s="190" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L15" s="191" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="M15" s="190" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="N15" s="186">
         <v>2</v>
       </c>
       <c r="O15" s="189" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="P15" s="189" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q15" s="192">
         <v>1</v>
@@ -9672,20 +9675,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C16" s="65" t="s">
         <v>130</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="O16" s="185"/>
       <c r="P16" s="185"/>
@@ -9696,18 +9699,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C17" s="65" t="s">
         <v>131</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E17" s="66"/>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -9716,20 +9719,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C18" s="65" t="s">
         <v>132</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E18" s="66" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -9738,13 +9741,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
@@ -9764,14 +9767,14 @@
         <v>128</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -9786,14 +9789,14 @@
         <v>129</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" thickBot="1">
@@ -9886,20 +9889,20 @@
         <v>2</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C29" s="204" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D29" s="205"/>
       <c r="E29" s="44" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F29" s="44" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G29" s="53" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" thickBot="1">
@@ -9941,7 +9944,7 @@
       <c r="A34" s="145"/>
       <c r="B34" s="146"/>
       <c r="C34" s="233" t="s">
-        <v>133</v>
+        <v>236</v>
       </c>
       <c r="D34" s="234"/>
       <c r="E34" s="233" t="s">
@@ -10049,8 +10052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -10118,7 +10121,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="224" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G4" s="225"/>
     </row>
@@ -10127,7 +10130,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="224" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D5" s="227"/>
       <c r="E5" s="42"/>
@@ -10139,7 +10142,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="224" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D6" s="227"/>
       <c r="E6" s="43"/>
@@ -10158,7 +10161,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="B8" s="211" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C8" s="212"/>
       <c r="D8" s="212"/>
@@ -10213,22 +10216,22 @@
         <v>31</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J13" s="13" t="s">
         <v>130</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>141</v>
+        <v>235</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="M13" s="13" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="O13" s="13" t="s">
         <v>128</v>
@@ -10266,7 +10269,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K14" s="13">
         <v>1</v>
@@ -10278,13 +10281,13 @@
         <v>1</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O14" s="185" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="P14" s="185" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q14" s="127"/>
       <c r="R14" s="127"/>
@@ -10296,13 +10299,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C15" s="65" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -10316,7 +10319,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K15" s="13">
         <v>2</v>
@@ -10331,10 +10334,10 @@
         <v>1</v>
       </c>
       <c r="O15" s="185" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="P15" s="185" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="Q15" s="127"/>
       <c r="R15" s="127"/>
@@ -10346,20 +10349,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -10369,20 +10372,20 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>234</v>
+      </c>
+      <c r="D17" s="65" t="s">
         <v>186</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>189</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -10391,10 +10394,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D18" s="129" t="s">
         <v>53</v>
@@ -10402,7 +10405,7 @@
       <c r="E18" s="66"/>
       <c r="F18" s="67"/>
       <c r="G18" s="117" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -10417,14 +10420,14 @@
         <v>128</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -10439,14 +10442,14 @@
         <v>129</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" thickBot="1">
@@ -10570,7 +10573,7 @@
       </c>
       <c r="B31" s="138"/>
       <c r="C31" s="230" t="s">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="D31" s="230"/>
       <c r="E31" s="230" t="s">
@@ -10587,7 +10590,7 @@
       </c>
       <c r="B32" s="161"/>
       <c r="C32" s="235" t="s">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="D32" s="235"/>
       <c r="E32" s="235" t="s">
@@ -10630,7 +10633,7 @@
       </c>
       <c r="D36" s="230"/>
       <c r="E36" s="230" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F36" s="230"/>
       <c r="G36" s="160"/>
@@ -10683,7 +10686,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:K15"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -10748,7 +10751,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="224" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G4" s="225"/>
     </row>
@@ -10757,7 +10760,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="224" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D5" s="227"/>
       <c r="E5" s="42"/>
@@ -10769,7 +10772,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="224" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D6" s="227"/>
       <c r="E6" s="43"/>
@@ -10788,7 +10791,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="B8" s="228" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C8" s="212"/>
       <c r="D8" s="212"/>
@@ -10846,10 +10849,10 @@
         <v>114</v>
       </c>
       <c r="J13" s="194" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K13" s="187" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L13" s="187" t="s">
         <v>128</v>
@@ -10886,16 +10889,16 @@
         <v>1</v>
       </c>
       <c r="J14" s="190" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K14" s="190" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="L14" s="189" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M14" s="189" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="N14" s="186">
         <v>1</v>
@@ -10907,13 +10910,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -10927,16 +10930,16 @@
         <v>2</v>
       </c>
       <c r="J15" s="190" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K15" s="186">
         <v>1</v>
       </c>
       <c r="L15" s="189" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M15" s="189" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="N15" s="186">
         <v>1</v>
@@ -10947,16 +10950,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D16" s="65" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="107"/>
@@ -10974,14 +10977,14 @@
         <v>128</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -10995,14 +10998,14 @@
         <v>129</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" thickBot="1">
@@ -11175,7 +11178,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:J17"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -11240,7 +11243,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="224" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G4" s="225"/>
     </row>
@@ -11249,7 +11252,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="224" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D5" s="227"/>
       <c r="E5" s="42"/>
@@ -11261,7 +11264,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="224" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D6" s="227"/>
       <c r="E6" s="43"/>
@@ -11280,7 +11283,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" s="228" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C8" s="212"/>
       <c r="D8" s="212"/>
@@ -11341,10 +11344,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="177" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C14" s="178" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="D14" s="178" t="s">
         <v>72</v>
@@ -11358,10 +11361,10 @@
       </c>
       <c r="H14" s="87"/>
       <c r="I14" s="187" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="J14" s="187" t="s">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="K14" s="136"/>
     </row>
@@ -11370,16 +11373,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="153" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C15" s="68" t="s">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F15" s="183"/>
       <c r="G15" s="184"/>
@@ -11501,11 +11504,11 @@
       <c r="A25" s="168"/>
       <c r="B25" s="169"/>
       <c r="C25" s="236" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="D25" s="237"/>
       <c r="E25" s="236" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F25" s="237"/>
       <c r="G25" s="167"/>
@@ -11514,11 +11517,11 @@
       <c r="A26" s="170"/>
       <c r="B26" s="171"/>
       <c r="C26" s="204" t="s">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="D26" s="238"/>
       <c r="E26" s="204" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F26" s="205"/>
       <c r="G26" s="172"/>

</xml_diff>

<commit_message>
System Design #20901: API Spec
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_Ver1.1_ANH_THANG_LE.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_Ver1.1_ANH_THANG_LE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER_MLD1\Google Drive\Git Mulodo\System Design 21912 Database Design\miniblog-le.thang\doc\backend\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER_MLD1\Google Drive\Git Mulodo\System Design 21914 API Specification\miniblog-le.thang\doc\backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7140" tabRatio="818" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7140" tabRatio="818" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -420,9 +420,6 @@
     <t>User Info</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -606,9 +603,6 @@
     <t>Just allow files in JPG, PNG, GIF, BMP.</t>
   </si>
   <si>
-    <t>0: male, 1: female</t>
-  </si>
-  <si>
     <t>Only allow standard format of email</t>
   </si>
   <si>
@@ -834,6 +828,12 @@
   </si>
   <si>
     <t>le.thangwef@moludo.com</t>
+  </si>
+  <si>
+    <t>0: male, 1: female, 2: ortrher</t>
+  </si>
+  <si>
+    <t>Title post</t>
   </si>
 </sst>
 </file>
@@ -920,35 +920,42 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -963,34 +970,40 @@
       <b/>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3941,6 +3954,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3951,12 +3967,78 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3972,93 +4054,27 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4096,9 +4112,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5794,29 +5807,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="195"/>
-      <c r="P13" s="195"/>
-      <c r="Q13" s="195"/>
-      <c r="R13" s="195"/>
-      <c r="S13" s="195"/>
-      <c r="T13" s="195"/>
-      <c r="U13" s="195"/>
-      <c r="V13" s="195"/>
-      <c r="W13" s="195"/>
-      <c r="X13" s="195"/>
-      <c r="Y13" s="195"/>
-      <c r="Z13" s="195"/>
-      <c r="AA13" s="195"/>
-      <c r="AB13" s="195"/>
-      <c r="AC13" s="195"/>
-      <c r="AD13" s="195"/>
-      <c r="AE13" s="195"/>
-      <c r="AF13" s="195"/>
-      <c r="AG13" s="195"/>
-      <c r="AH13" s="195"/>
-      <c r="AI13" s="195"/>
-      <c r="AJ13" s="195"/>
-      <c r="AK13" s="195"/>
+      <c r="O13" s="196"/>
+      <c r="P13" s="196"/>
+      <c r="Q13" s="196"/>
+      <c r="R13" s="196"/>
+      <c r="S13" s="196"/>
+      <c r="T13" s="196"/>
+      <c r="U13" s="196"/>
+      <c r="V13" s="196"/>
+      <c r="W13" s="196"/>
+      <c r="X13" s="196"/>
+      <c r="Y13" s="196"/>
+      <c r="Z13" s="196"/>
+      <c r="AA13" s="196"/>
+      <c r="AB13" s="196"/>
+      <c r="AC13" s="196"/>
+      <c r="AD13" s="196"/>
+      <c r="AE13" s="196"/>
+      <c r="AF13" s="196"/>
+      <c r="AG13" s="196"/>
+      <c r="AH13" s="196"/>
+      <c r="AI13" s="196"/>
+      <c r="AJ13" s="196"/>
+      <c r="AK13" s="196"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5848,29 +5861,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="195"/>
-      <c r="P14" s="195"/>
-      <c r="Q14" s="195"/>
-      <c r="R14" s="195"/>
-      <c r="S14" s="195"/>
-      <c r="T14" s="195"/>
-      <c r="U14" s="195"/>
-      <c r="V14" s="195"/>
-      <c r="W14" s="195"/>
-      <c r="X14" s="195"/>
-      <c r="Y14" s="195"/>
-      <c r="Z14" s="195"/>
-      <c r="AA14" s="195"/>
-      <c r="AB14" s="195"/>
-      <c r="AC14" s="195"/>
-      <c r="AD14" s="195"/>
-      <c r="AE14" s="195"/>
-      <c r="AF14" s="195"/>
-      <c r="AG14" s="195"/>
-      <c r="AH14" s="195"/>
-      <c r="AI14" s="195"/>
-      <c r="AJ14" s="195"/>
-      <c r="AK14" s="195"/>
+      <c r="O14" s="196"/>
+      <c r="P14" s="196"/>
+      <c r="Q14" s="196"/>
+      <c r="R14" s="196"/>
+      <c r="S14" s="196"/>
+      <c r="T14" s="196"/>
+      <c r="U14" s="196"/>
+      <c r="V14" s="196"/>
+      <c r="W14" s="196"/>
+      <c r="X14" s="196"/>
+      <c r="Y14" s="196"/>
+      <c r="Z14" s="196"/>
+      <c r="AA14" s="196"/>
+      <c r="AB14" s="196"/>
+      <c r="AC14" s="196"/>
+      <c r="AD14" s="196"/>
+      <c r="AE14" s="196"/>
+      <c r="AF14" s="196"/>
+      <c r="AG14" s="196"/>
+      <c r="AH14" s="196"/>
+      <c r="AI14" s="196"/>
+      <c r="AJ14" s="196"/>
+      <c r="AK14" s="196"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5898,43 +5911,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="L15" s="196"/>
-      <c r="M15" s="196"/>
-      <c r="N15" s="196"/>
-      <c r="O15" s="196"/>
-      <c r="P15" s="196"/>
-      <c r="Q15" s="196"/>
-      <c r="R15" s="196"/>
-      <c r="S15" s="196"/>
-      <c r="T15" s="196"/>
-      <c r="U15" s="196"/>
-      <c r="V15" s="196"/>
-      <c r="W15" s="196"/>
-      <c r="X15" s="196"/>
-      <c r="Y15" s="196"/>
-      <c r="Z15" s="196"/>
-      <c r="AA15" s="196"/>
-      <c r="AB15" s="196"/>
-      <c r="AC15" s="196"/>
-      <c r="AD15" s="196"/>
-      <c r="AE15" s="196"/>
-      <c r="AF15" s="196"/>
-      <c r="AG15" s="196"/>
-      <c r="AH15" s="196"/>
-      <c r="AI15" s="196"/>
-      <c r="AJ15" s="196"/>
-      <c r="AK15" s="196"/>
-      <c r="AL15" s="196"/>
-      <c r="AM15" s="196"/>
-      <c r="AN15" s="196"/>
-      <c r="AO15" s="196"/>
-      <c r="AP15" s="196"/>
-      <c r="AQ15" s="196"/>
-      <c r="AR15" s="196"/>
-      <c r="AS15" s="196"/>
+      <c r="K15" s="197" t="s">
+        <v>118</v>
+      </c>
+      <c r="L15" s="197"/>
+      <c r="M15" s="197"/>
+      <c r="N15" s="197"/>
+      <c r="O15" s="197"/>
+      <c r="P15" s="197"/>
+      <c r="Q15" s="197"/>
+      <c r="R15" s="197"/>
+      <c r="S15" s="197"/>
+      <c r="T15" s="197"/>
+      <c r="U15" s="197"/>
+      <c r="V15" s="197"/>
+      <c r="W15" s="197"/>
+      <c r="X15" s="197"/>
+      <c r="Y15" s="197"/>
+      <c r="Z15" s="197"/>
+      <c r="AA15" s="197"/>
+      <c r="AB15" s="197"/>
+      <c r="AC15" s="197"/>
+      <c r="AD15" s="197"/>
+      <c r="AE15" s="197"/>
+      <c r="AF15" s="197"/>
+      <c r="AG15" s="197"/>
+      <c r="AH15" s="197"/>
+      <c r="AI15" s="197"/>
+      <c r="AJ15" s="197"/>
+      <c r="AK15" s="197"/>
+      <c r="AL15" s="197"/>
+      <c r="AM15" s="197"/>
+      <c r="AN15" s="197"/>
+      <c r="AO15" s="197"/>
+      <c r="AP15" s="197"/>
+      <c r="AQ15" s="197"/>
+      <c r="AR15" s="197"/>
+      <c r="AS15" s="197"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5954,41 +5967,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="196"/>
-      <c r="L16" s="196"/>
-      <c r="M16" s="196"/>
-      <c r="N16" s="196"/>
-      <c r="O16" s="196"/>
-      <c r="P16" s="196"/>
-      <c r="Q16" s="196"/>
-      <c r="R16" s="196"/>
-      <c r="S16" s="196"/>
-      <c r="T16" s="196"/>
-      <c r="U16" s="196"/>
-      <c r="V16" s="196"/>
-      <c r="W16" s="196"/>
-      <c r="X16" s="196"/>
-      <c r="Y16" s="196"/>
-      <c r="Z16" s="196"/>
-      <c r="AA16" s="196"/>
-      <c r="AB16" s="196"/>
-      <c r="AC16" s="196"/>
-      <c r="AD16" s="196"/>
-      <c r="AE16" s="196"/>
-      <c r="AF16" s="196"/>
-      <c r="AG16" s="196"/>
-      <c r="AH16" s="196"/>
-      <c r="AI16" s="196"/>
-      <c r="AJ16" s="196"/>
-      <c r="AK16" s="196"/>
-      <c r="AL16" s="196"/>
-      <c r="AM16" s="196"/>
-      <c r="AN16" s="196"/>
-      <c r="AO16" s="196"/>
-      <c r="AP16" s="196"/>
-      <c r="AQ16" s="196"/>
-      <c r="AR16" s="196"/>
-      <c r="AS16" s="196"/>
+      <c r="K16" s="197"/>
+      <c r="L16" s="197"/>
+      <c r="M16" s="197"/>
+      <c r="N16" s="197"/>
+      <c r="O16" s="197"/>
+      <c r="P16" s="197"/>
+      <c r="Q16" s="197"/>
+      <c r="R16" s="197"/>
+      <c r="S16" s="197"/>
+      <c r="T16" s="197"/>
+      <c r="U16" s="197"/>
+      <c r="V16" s="197"/>
+      <c r="W16" s="197"/>
+      <c r="X16" s="197"/>
+      <c r="Y16" s="197"/>
+      <c r="Z16" s="197"/>
+      <c r="AA16" s="197"/>
+      <c r="AB16" s="197"/>
+      <c r="AC16" s="197"/>
+      <c r="AD16" s="197"/>
+      <c r="AE16" s="197"/>
+      <c r="AF16" s="197"/>
+      <c r="AG16" s="197"/>
+      <c r="AH16" s="197"/>
+      <c r="AI16" s="197"/>
+      <c r="AJ16" s="197"/>
+      <c r="AK16" s="197"/>
+      <c r="AL16" s="197"/>
+      <c r="AM16" s="197"/>
+      <c r="AN16" s="197"/>
+      <c r="AO16" s="197"/>
+      <c r="AP16" s="197"/>
+      <c r="AQ16" s="197"/>
+      <c r="AR16" s="197"/>
+      <c r="AS16" s="197"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6577,14 +6590,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="197">
+      <c r="AN27" s="198">
         <v>42310</v>
       </c>
-      <c r="AO27" s="197"/>
-      <c r="AP27" s="197"/>
-      <c r="AQ27" s="197"/>
-      <c r="AR27" s="197"/>
-      <c r="AS27" s="197"/>
+      <c r="AO27" s="198"/>
+      <c r="AP27" s="198"/>
+      <c r="AQ27" s="198"/>
+      <c r="AR27" s="198"/>
+      <c r="AS27" s="198"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7074,105 +7087,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
+      <c r="C2" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="226"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
+      <c r="F2" s="200" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="221"/>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="224" t="s">
+      <c r="F3" s="202" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="225"/>
+      <c r="G3" s="207"/>
     </row>
     <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
+      <c r="C4" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="227"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
+      <c r="C5" s="202" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="227"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="202" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="227"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:7" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="228" t="s">
+      <c r="B8" s="235" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -7277,10 +7290,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="206" t="s">
+      <c r="C19" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="207"/>
+      <c r="D19" s="209"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -7298,10 +7311,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="218" t="s">
+      <c r="C20" s="222" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="219"/>
+      <c r="D20" s="223"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -7315,10 +7328,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="239" t="s">
+      <c r="C21" s="240" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="240"/>
+      <c r="D21" s="241"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -7337,14 +7350,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="199" t="s">
+      <c r="C24" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="200"/>
-      <c r="E24" s="199" t="s">
+      <c r="D24" s="211"/>
+      <c r="E24" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="201"/>
+      <c r="F24" s="224"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -7361,14 +7374,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="199" t="s">
+      <c r="C27" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="200"/>
-      <c r="E27" s="199" t="s">
+      <c r="D27" s="211"/>
+      <c r="E27" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="201"/>
+      <c r="F27" s="224"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -7378,14 +7391,23 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="239"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="241"/>
-      <c r="F28" s="242"/>
+      <c r="C28" s="240"/>
+      <c r="D28" s="241"/>
+      <c r="E28" s="242"/>
+      <c r="F28" s="243"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -7398,15 +7420,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7454,103 +7467,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
+      <c r="C2" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="226"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="245" t="s">
+      <c r="F2" s="246" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="246"/>
+      <c r="G2" s="247"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="247" t="s">
+      <c r="F3" s="248" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="225"/>
+      <c r="G3" s="207"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
+      <c r="C4" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="227"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
+      <c r="C5" s="202" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="227"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="202" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="227"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="228"/>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="235"/>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -7766,10 +7779,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="206" t="s">
+      <c r="C21" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="207"/>
+      <c r="D21" s="209"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -7793,10 +7806,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="218" t="s">
+      <c r="C22" s="222" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="219"/>
+      <c r="D22" s="223"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -7816,10 +7829,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="204" t="s">
+      <c r="C23" s="227" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="205"/>
+      <c r="D23" s="228"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -7837,10 +7850,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="239" t="s">
+      <c r="C24" s="240" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="240"/>
+      <c r="D24" s="241"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -7879,14 +7892,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="199" t="s">
+      <c r="C27" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="200"/>
-      <c r="E27" s="199" t="s">
+      <c r="D27" s="211"/>
+      <c r="E27" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="201"/>
+      <c r="F27" s="224"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -7923,14 +7936,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="199" t="s">
+      <c r="C30" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="200"/>
-      <c r="E30" s="199" t="s">
+      <c r="D30" s="211"/>
+      <c r="E30" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="201"/>
+      <c r="F30" s="224"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -7946,14 +7959,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="218" t="s">
+      <c r="C31" s="222" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="219"/>
-      <c r="E31" s="204" t="s">
+      <c r="D31" s="223"/>
+      <c r="E31" s="227" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="205"/>
+      <c r="F31" s="228"/>
       <c r="G31" s="53" t="s">
         <v>77</v>
       </c>
@@ -7969,14 +7982,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="243" t="s">
+      <c r="C32" s="244" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="244"/>
-      <c r="E32" s="241" t="s">
+      <c r="D32" s="245"/>
+      <c r="E32" s="242" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="242"/>
+      <c r="F32" s="243"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -8029,14 +8042,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -8053,6 +8058,14 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8116,7 +8129,7 @@
         <v>102</v>
       </c>
       <c r="D3" s="94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="95" t="s">
         <v>100</v>
@@ -8126,13 +8139,13 @@
     <row r="4" spans="2:6">
       <c r="B4" s="97"/>
       <c r="C4" s="114" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D4" s="94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="99" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F4" s="100"/>
     </row>
@@ -8377,11 +8390,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" thickBot="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -8402,7 +8415,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="130" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8411,10 +8424,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="123" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -8423,10 +8436,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8435,10 +8448,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="123" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="124" t="s">
         <v>140</v>
-      </c>
-      <c r="C6" s="124" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8447,7 +8460,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="123" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C7" s="124"/>
     </row>
@@ -8648,14 +8661,14 @@
   </sheetPr>
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="18" hidden="1" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" style="18" customWidth="1"/>
     <col min="5" max="6" width="10.140625" style="18" customWidth="1"/>
     <col min="7" max="7" width="45" style="18" customWidth="1"/>
@@ -8681,114 +8694,114 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="226"/>
+      <c r="C2" s="200" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="221"/>
+      <c r="F2" s="200" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:21" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="222">
+      <c r="F3" s="205">
         <v>42249</v>
       </c>
-      <c r="G3" s="223"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:21" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="227"/>
+      <c r="C4" s="202" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:21" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
+      <c r="C5" s="202" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="227"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:21" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="202" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="227"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:21" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:21" ht="12" customHeight="1">
-      <c r="B8" s="211" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="215" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:21" ht="12" customHeight="1">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:21" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -8814,40 +8827,40 @@
         <v>31</v>
       </c>
       <c r="I13" s="194" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J13" s="194" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K13" s="194" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L13" s="187" t="s">
+        <v>137</v>
+      </c>
+      <c r="M13" s="187" t="s">
         <v>138</v>
       </c>
-      <c r="M13" s="187" t="s">
-        <v>139</v>
-      </c>
       <c r="N13" s="187" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O13" s="187" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P13" s="187" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q13" s="187" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R13" s="194" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="S13" s="194" t="s">
+        <v>127</v>
+      </c>
+      <c r="T13" s="194" t="s">
         <v>128</v>
-      </c>
-      <c r="T13" s="194" t="s">
-        <v>129</v>
       </c>
       <c r="U13" s="194" t="s">
         <v>6</v>
@@ -8858,13 +8871,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -8878,36 +8891,36 @@
         <v>1</v>
       </c>
       <c r="J14" s="186" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" s="186" t="s">
         <v>110</v>
       </c>
-      <c r="K14" s="186" t="s">
-        <v>111</v>
-      </c>
       <c r="L14" s="186" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M14" s="186" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N14" s="186">
         <v>0</v>
       </c>
       <c r="O14" s="186" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P14" s="191" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q14" s="191" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R14" s="186">
         <v>11000</v>
       </c>
-      <c r="S14" s="248">
+      <c r="S14" s="195">
         <v>41922.465277777781</v>
       </c>
-      <c r="T14" s="248">
+      <c r="T14" s="195">
         <v>41922.465277777781</v>
       </c>
       <c r="U14" s="186">
@@ -8920,10 +8933,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" s="65" t="s">
         <v>55</v>
@@ -8933,43 +8946,43 @@
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="186">
         <v>2</v>
       </c>
       <c r="J15" s="186" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="186" t="s">
         <v>112</v>
       </c>
-      <c r="K15" s="186" t="s">
-        <v>113</v>
-      </c>
       <c r="L15" s="186" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M15" s="186" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N15" s="186">
         <v>1</v>
       </c>
       <c r="O15" s="186" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P15" s="191" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q15" s="191" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R15" s="186">
         <v>11000</v>
       </c>
-      <c r="S15" s="248">
+      <c r="S15" s="195">
         <v>41922.46875</v>
       </c>
-      <c r="T15" s="248">
+      <c r="T15" s="195">
         <v>41922.46875</v>
       </c>
       <c r="U15" s="186">
@@ -8982,56 +8995,56 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>55</v>
+        <v>169</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H16" s="87"/>
       <c r="I16" s="186">
         <v>3</v>
       </c>
       <c r="J16" s="186" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K16" s="186" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L16" s="186" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M16" s="186" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N16" s="186">
         <v>2</v>
       </c>
       <c r="O16" s="186" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="P16" s="191" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q16" s="191" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R16" s="186">
         <v>11110</v>
       </c>
-      <c r="S16" s="248">
+      <c r="S16" s="195">
         <v>41922.472222222219</v>
       </c>
-      <c r="T16" s="248">
+      <c r="T16" s="195">
         <v>41922.472222222219</v>
       </c>
       <c r="U16" s="186">
@@ -9044,55 +9057,55 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I17" s="186">
         <v>4</v>
       </c>
       <c r="J17" s="186" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K17" s="186" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L17" s="186" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M17" s="186" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N17" s="186">
         <v>3</v>
       </c>
       <c r="O17" s="186" t="s">
+        <v>237</v>
+      </c>
+      <c r="P17" s="191" t="s">
         <v>239</v>
       </c>
-      <c r="P17" s="191" t="s">
-        <v>241</v>
-      </c>
       <c r="Q17" s="191" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R17" s="186">
         <v>11111</v>
       </c>
-      <c r="S17" s="248">
+      <c r="S17" s="195">
         <v>41922.475694444445</v>
       </c>
-      <c r="T17" s="248">
+      <c r="T17" s="195">
         <v>41922.475694444445</v>
       </c>
       <c r="U17" s="186">
@@ -9105,20 +9118,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="117" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -9127,20 +9140,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -9149,13 +9162,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
@@ -9164,7 +9177,7 @@
         <v>99</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -9173,22 +9186,22 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D21" s="129" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="F21" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="G21" s="106" t="s">
         <v>178</v>
-      </c>
-      <c r="E21" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" s="67" t="s">
-        <v>179</v>
-      </c>
-      <c r="G21" s="106" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15">
@@ -9197,20 +9210,20 @@
         <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E22" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="67"/>
       <c r="G22" s="106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H22" s="136"/>
     </row>
@@ -9220,20 +9233,20 @@
         <v>10</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D23" s="129" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E23" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F23" s="67"/>
       <c r="G23" s="106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -9242,20 +9255,20 @@
         <v>11</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E24" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="67"/>
       <c r="G24" s="106" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -9267,17 +9280,17 @@
         <v>41</v>
       </c>
       <c r="C25" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E25" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="67"/>
       <c r="G25" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -9289,17 +9302,17 @@
         <v>41</v>
       </c>
       <c r="C26" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E26" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="67"/>
       <c r="G26" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="12.75" thickBot="1">
@@ -9314,16 +9327,16 @@
         <v>6</v>
       </c>
       <c r="D27" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E27" s="155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F27" s="158" t="s">
         <v>99</v>
       </c>
       <c r="G27" s="156" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -9341,10 +9354,10 @@
       <c r="B30" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="206" t="s">
+      <c r="C30" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="207"/>
+      <c r="D30" s="209"/>
       <c r="E30" s="34" t="s">
         <v>33</v>
       </c>
@@ -9362,10 +9375,10 @@
       <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="218" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="219"/>
+      <c r="C31" s="222" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="223"/>
       <c r="E31" s="46" t="s">
         <v>3</v>
       </c>
@@ -9379,20 +9392,20 @@
         <v>2</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="204" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" s="205"/>
+        <v>143</v>
+      </c>
+      <c r="C32" s="227" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="228"/>
       <c r="E32" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
@@ -9400,8 +9413,8 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="202"/>
-      <c r="D33" s="203"/>
+      <c r="C33" s="225"/>
+      <c r="D33" s="226"/>
       <c r="E33" s="58"/>
       <c r="F33" s="58"/>
       <c r="G33" s="55"/>
@@ -9418,14 +9431,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="199" t="s">
+      <c r="C36" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="200"/>
-      <c r="E36" s="199" t="s">
+      <c r="D36" s="211"/>
+      <c r="E36" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="201"/>
+      <c r="F36" s="224"/>
       <c r="G36" s="38" t="s">
         <v>38</v>
       </c>
@@ -9442,40 +9455,40 @@
       <c r="B41" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="199" t="s">
+      <c r="C41" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="200"/>
-      <c r="E41" s="199" t="s">
+      <c r="D41" s="211"/>
+      <c r="E41" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="201"/>
+      <c r="F41" s="224"/>
       <c r="G41" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -9506,8 +9519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:D34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -9537,108 +9550,108 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="226"/>
+      <c r="C2" s="200" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="221"/>
+      <c r="F2" s="200" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:18" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="222">
+      <c r="F3" s="205">
         <f ca="1" xml:space="preserve"> TODAY()</f>
-        <v>42046</v>
-      </c>
-      <c r="G3" s="223"/>
+        <v>42047</v>
+      </c>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:18" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="227"/>
+      <c r="C4" s="202" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:18" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="227"/>
+      <c r="C5" s="202" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:18" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="227"/>
+      <c r="C6" s="202" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:18" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="228" t="s">
-        <v>199</v>
-      </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="235" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:18" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:18" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9668,7 +9681,7 @@
         <v>31</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P13" s="128"/>
       <c r="Q13" s="128"/>
@@ -9679,13 +9692,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -9695,28 +9708,28 @@
         <v>50</v>
       </c>
       <c r="I14" s="186" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J14" s="187" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="187" t="s">
+        <v>129</v>
+      </c>
+      <c r="L14" s="187" t="s">
+        <v>130</v>
+      </c>
+      <c r="M14" s="187" t="s">
+        <v>131</v>
+      </c>
+      <c r="N14" s="187" t="s">
+        <v>233</v>
+      </c>
+      <c r="O14" s="186" t="s">
         <v>127</v>
       </c>
-      <c r="K14" s="187" t="s">
-        <v>130</v>
-      </c>
-      <c r="L14" s="187" t="s">
-        <v>131</v>
-      </c>
-      <c r="M14" s="187" t="s">
-        <v>132</v>
-      </c>
-      <c r="N14" s="187" t="s">
-        <v>235</v>
-      </c>
-      <c r="O14" s="186" t="s">
+      <c r="P14" s="186" t="s">
         <v>128</v>
-      </c>
-      <c r="P14" s="186" t="s">
-        <v>129</v>
       </c>
       <c r="Q14" s="188" t="s">
         <v>6</v>
@@ -9728,44 +9741,44 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>106</v>
+        <v>242</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15" s="186">
         <v>1</v>
       </c>
       <c r="J15" s="190" t="s">
+        <v>217</v>
+      </c>
+      <c r="K15" s="190" t="s">
+        <v>218</v>
+      </c>
+      <c r="L15" s="191" t="s">
         <v>219</v>
       </c>
-      <c r="K15" s="190" t="s">
-        <v>220</v>
-      </c>
-      <c r="L15" s="191" t="s">
-        <v>221</v>
-      </c>
       <c r="M15" s="190" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N15" s="186">
         <v>2</v>
       </c>
       <c r="O15" s="189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P15" s="189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q15" s="192">
         <v>1</v>
@@ -9777,20 +9790,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O16" s="185"/>
       <c r="P16" s="185"/>
@@ -9801,18 +9814,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E17" s="66"/>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -9821,20 +9834,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E18" s="66" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -9843,13 +9856,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
@@ -9866,17 +9879,17 @@
         <v>41</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -9888,17 +9901,17 @@
         <v>42</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" thickBot="1">
@@ -9913,7 +9926,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="133" t="s">
         <v>3</v>
@@ -9922,7 +9935,7 @@
         <v>99</v>
       </c>
       <c r="G22" s="134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -9953,10 +9966,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="206" t="s">
+      <c r="C27" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="207"/>
+      <c r="D27" s="209"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -9974,10 +9987,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="218" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="219"/>
+      <c r="C28" s="222" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="223"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -9991,20 +10004,20 @@
         <v>2</v>
       </c>
       <c r="B29" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="227" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="204" t="s">
+      <c r="D29" s="228"/>
+      <c r="E29" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" s="53" t="s">
         <v>145</v>
-      </c>
-      <c r="D29" s="205"/>
-      <c r="E29" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="G29" s="53" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" thickBot="1">
@@ -10012,8 +10025,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="202"/>
-      <c r="D30" s="203"/>
+      <c r="C30" s="225"/>
+      <c r="D30" s="226"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="28"/>
@@ -10030,14 +10043,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="199" t="s">
+      <c r="C33" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="200"/>
-      <c r="E33" s="199" t="s">
+      <c r="D33" s="211"/>
+      <c r="E33" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="201"/>
+      <c r="F33" s="224"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -10046,15 +10059,15 @@
       <c r="A34" s="145"/>
       <c r="B34" s="146"/>
       <c r="C34" s="233" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D34" s="234"/>
       <c r="E34" s="233" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F34" s="234"/>
       <c r="G34" s="150" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H34" s="137"/>
     </row>
@@ -10085,14 +10098,14 @@
       <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="199" t="s">
+      <c r="C38" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="200"/>
-      <c r="E38" s="199" t="s">
+      <c r="D38" s="211"/>
+      <c r="E38" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="201"/>
+      <c r="F38" s="224"/>
       <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
@@ -10101,15 +10114,15 @@
       <c r="A39" s="140"/>
       <c r="B39" s="139"/>
       <c r="C39" s="229" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" s="230"/>
       <c r="E39" s="231" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F39" s="232"/>
       <c r="G39" s="141" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -10118,6 +10131,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="C38:D38"/>
@@ -10130,18 +10155,6 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L15" r:id="rId1"/>
@@ -10185,114 +10198,114 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="226"/>
+      <c r="C2" s="200" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="221"/>
+      <c r="F2" s="200" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:20" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="222">
+      <c r="F3" s="205">
         <v>42045</v>
       </c>
-      <c r="G3" s="223"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:20" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="227"/>
+      <c r="C4" s="202" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:20" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="227"/>
+      <c r="C5" s="202" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:20" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" s="227"/>
+      <c r="C6" s="202" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:20" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="B8" s="211" t="s">
-        <v>200</v>
-      </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="215" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:20" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:20" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -10318,28 +10331,28 @@
         <v>31</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M13" s="13" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O13" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" s="13" t="s">
         <v>128</v>
-      </c>
-      <c r="P13" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="Q13" s="128"/>
       <c r="R13" s="128"/>
@@ -10351,10 +10364,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>53</v>
@@ -10371,7 +10384,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K14" s="13">
         <v>1</v>
@@ -10386,10 +10399,10 @@
         <v>0</v>
       </c>
       <c r="O14" s="185" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P14" s="185" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q14" s="127"/>
       <c r="R14" s="127"/>
@@ -10401,27 +10414,27 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="13">
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K15" s="13">
         <v>2</v>
@@ -10436,10 +10449,10 @@
         <v>1</v>
       </c>
       <c r="O15" s="185" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P15" s="185" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Q15" s="127"/>
       <c r="R15" s="127"/>
@@ -10451,20 +10464,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -10474,20 +10487,20 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -10496,10 +10509,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D18" s="129" t="s">
         <v>53</v>
@@ -10507,7 +10520,7 @@
       <c r="E18" s="66"/>
       <c r="F18" s="67"/>
       <c r="G18" s="117" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -10519,17 +10532,17 @@
         <v>41</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -10541,17 +10554,17 @@
         <v>42</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" thickBot="1">
@@ -10566,7 +10579,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="133" t="s">
         <v>3</v>
@@ -10575,7 +10588,7 @@
         <v>99</v>
       </c>
       <c r="G21" s="134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" thickBot="1">
@@ -10590,10 +10603,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="206" t="s">
+      <c r="C24" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="207"/>
+      <c r="D24" s="209"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -10611,10 +10624,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="218" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="219"/>
+      <c r="C25" s="222" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="223"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -10628,8 +10641,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="51"/>
-      <c r="C26" s="204"/>
-      <c r="D26" s="205"/>
+      <c r="C26" s="227"/>
+      <c r="D26" s="228"/>
       <c r="E26" s="52"/>
       <c r="F26" s="52"/>
       <c r="G26" s="53"/>
@@ -10639,8 +10652,8 @@
         <v>3</v>
       </c>
       <c r="B27" s="54"/>
-      <c r="C27" s="202"/>
-      <c r="D27" s="203"/>
+      <c r="C27" s="225"/>
+      <c r="D27" s="226"/>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
       <c r="G27" s="55"/>
@@ -10657,14 +10670,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="199" t="s">
+      <c r="C30" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="200"/>
-      <c r="E30" s="199" t="s">
+      <c r="D30" s="211"/>
+      <c r="E30" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="201"/>
+      <c r="F30" s="224"/>
       <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
@@ -10675,15 +10688,15 @@
       </c>
       <c r="B31" s="138"/>
       <c r="C31" s="230" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D31" s="230"/>
       <c r="E31" s="230" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F31" s="230"/>
       <c r="G31" s="160" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="12.75" thickBot="1">
@@ -10691,16 +10704,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="161"/>
-      <c r="C32" s="235" t="s">
-        <v>233</v>
-      </c>
-      <c r="D32" s="235"/>
-      <c r="E32" s="235" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="235"/>
+      <c r="C32" s="236" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="236"/>
+      <c r="E32" s="236" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="236"/>
       <c r="G32" s="149" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" thickBot="1">
@@ -10715,14 +10728,14 @@
       <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="199" t="s">
+      <c r="C35" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="200"/>
-      <c r="E35" s="199" t="s">
+      <c r="D35" s="211"/>
+      <c r="E35" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="201"/>
+      <c r="F35" s="224"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
@@ -10731,11 +10744,11 @@
       <c r="A36" s="159"/>
       <c r="B36" s="138"/>
       <c r="C36" s="230" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="230"/>
       <c r="E36" s="230" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F36" s="230"/>
       <c r="G36" s="160"/>
@@ -10751,6 +10764,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C35:D35"/>
@@ -10765,18 +10790,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10815,114 +10828,114 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="226"/>
+      <c r="C2" s="200" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="221"/>
+      <c r="F2" s="200" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="222">
+      <c r="F3" s="205">
         <v>42279</v>
       </c>
-      <c r="G3" s="223"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="227"/>
+      <c r="C4" s="202" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="227"/>
+      <c r="C5" s="202" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="227"/>
+      <c r="C6" s="202" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="228" t="s">
-        <v>201</v>
-      </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="235" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:14" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -10948,19 +10961,19 @@
         <v>31</v>
       </c>
       <c r="I13" s="194" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J13" s="194" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K13" s="187" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L13" s="187" t="s">
+        <v>127</v>
+      </c>
+      <c r="M13" s="187" t="s">
         <v>128</v>
-      </c>
-      <c r="M13" s="187" t="s">
-        <v>129</v>
       </c>
       <c r="N13" s="193" t="s">
         <v>6</v>
@@ -10971,10 +10984,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>72</v>
@@ -10991,16 +11004,16 @@
         <v>1</v>
       </c>
       <c r="J14" s="190" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K14" s="190">
         <v>0</v>
       </c>
       <c r="L14" s="189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M14" s="189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N14" s="186">
         <v>1</v>
@@ -11012,36 +11025,36 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="186">
         <v>2</v>
       </c>
       <c r="J15" s="190" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K15" s="186">
         <v>1</v>
       </c>
       <c r="L15" s="189" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M15" s="189" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N15" s="186">
         <v>1</v>
@@ -11052,16 +11065,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D16" s="65" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="107"/>
@@ -11076,17 +11089,17 @@
         <v>41</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -11097,17 +11110,17 @@
         <v>42</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" thickBot="1">
@@ -11121,7 +11134,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="133" t="s">
         <v>3</v>
@@ -11130,7 +11143,7 @@
         <v>99</v>
       </c>
       <c r="G19" s="134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" thickBot="1">
@@ -11145,10 +11158,10 @@
       <c r="B22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="206" t="s">
+      <c r="C22" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="207"/>
+      <c r="D22" s="209"/>
       <c r="E22" s="34" t="s">
         <v>33</v>
       </c>
@@ -11166,10 +11179,10 @@
       <c r="B23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="218" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="219"/>
+      <c r="C23" s="222" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="223"/>
       <c r="E23" s="46" t="s">
         <v>3</v>
       </c>
@@ -11183,8 +11196,8 @@
         <v>2</v>
       </c>
       <c r="B24" s="51"/>
-      <c r="C24" s="204"/>
-      <c r="D24" s="205"/>
+      <c r="C24" s="227"/>
+      <c r="D24" s="228"/>
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
       <c r="G24" s="53"/>
@@ -11194,8 +11207,8 @@
         <v>3</v>
       </c>
       <c r="B25" s="54"/>
-      <c r="C25" s="202"/>
-      <c r="D25" s="203"/>
+      <c r="C25" s="225"/>
+      <c r="D25" s="226"/>
       <c r="E25" s="58"/>
       <c r="F25" s="58"/>
       <c r="G25" s="55"/>
@@ -11212,14 +11225,14 @@
       <c r="B28" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="199" t="s">
+      <c r="C28" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="200"/>
-      <c r="E28" s="199" t="s">
+      <c r="D28" s="211"/>
+      <c r="E28" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="201"/>
+      <c r="F28" s="224"/>
       <c r="G28" s="38" t="s">
         <v>38</v>
       </c>
@@ -11236,28 +11249,20 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="199" t="s">
+      <c r="C32" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="200"/>
-      <c r="E32" s="199" t="s">
+      <c r="D32" s="211"/>
+      <c r="E32" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="201"/>
+      <c r="F32" s="224"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -11270,6 +11275,14 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11307,107 +11320,107 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="226"/>
+      <c r="C2" s="200" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="221"/>
+      <c r="F2" s="200" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:12" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="222">
+      <c r="F3" s="205">
         <v>42279</v>
       </c>
-      <c r="G3" s="223"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:12" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="227"/>
+      <c r="C4" s="202" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:12" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" s="227"/>
+      <c r="C5" s="202" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:12" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
-        <v>205</v>
-      </c>
-      <c r="D6" s="227"/>
+      <c r="C6" s="202" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:12" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="228" t="s">
-        <v>202</v>
-      </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="235" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11437,7 +11450,7 @@
         <v>31</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L13" s="128"/>
     </row>
@@ -11446,10 +11459,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="177" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C14" s="178" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D14" s="178" t="s">
         <v>72</v>
@@ -11459,14 +11472,14 @@
       </c>
       <c r="F14" s="180"/>
       <c r="G14" s="181" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H14" s="87"/>
       <c r="I14" s="187" t="s">
+        <v>229</v>
+      </c>
+      <c r="J14" s="187" t="s">
         <v>231</v>
-      </c>
-      <c r="J14" s="187" t="s">
-        <v>233</v>
       </c>
       <c r="K14" s="136"/>
     </row>
@@ -11475,16 +11488,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="153" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C15" s="68" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F15" s="183"/>
       <c r="G15" s="184"/>
@@ -11523,10 +11536,10 @@
       <c r="B18" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="206" t="s">
+      <c r="C18" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="207"/>
+      <c r="D18" s="209"/>
       <c r="E18" s="34" t="s">
         <v>33</v>
       </c>
@@ -11544,10 +11557,10 @@
       <c r="B19" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="218" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="219"/>
+      <c r="C19" s="222" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="223"/>
       <c r="E19" s="46" t="s">
         <v>3</v>
       </c>
@@ -11561,8 +11574,8 @@
         <v>2</v>
       </c>
       <c r="B20" s="51"/>
-      <c r="C20" s="204"/>
-      <c r="D20" s="205"/>
+      <c r="C20" s="227"/>
+      <c r="D20" s="228"/>
       <c r="E20" s="52"/>
       <c r="F20" s="52"/>
       <c r="G20" s="53"/>
@@ -11572,8 +11585,8 @@
         <v>3</v>
       </c>
       <c r="B21" s="54"/>
-      <c r="C21" s="202"/>
-      <c r="D21" s="203"/>
+      <c r="C21" s="225"/>
+      <c r="D21" s="226"/>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
       <c r="G21" s="55"/>
@@ -11590,14 +11603,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="199" t="s">
+      <c r="C24" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="200"/>
-      <c r="E24" s="199" t="s">
+      <c r="D24" s="211"/>
+      <c r="E24" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="201"/>
+      <c r="F24" s="224"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -11605,27 +11618,27 @@
     <row r="25" spans="1:10">
       <c r="A25" s="168"/>
       <c r="B25" s="169"/>
-      <c r="C25" s="236" t="s">
-        <v>231</v>
-      </c>
-      <c r="D25" s="237"/>
-      <c r="E25" s="236" t="s">
-        <v>206</v>
-      </c>
-      <c r="F25" s="237"/>
+      <c r="C25" s="237" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="238"/>
+      <c r="E25" s="237" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="238"/>
       <c r="G25" s="167"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="170"/>
       <c r="B26" s="171"/>
-      <c r="C26" s="204" t="s">
-        <v>232</v>
-      </c>
-      <c r="D26" s="238"/>
-      <c r="E26" s="204" t="s">
-        <v>207</v>
-      </c>
-      <c r="F26" s="205"/>
+      <c r="C26" s="227" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="239"/>
+      <c r="E26" s="227" t="s">
+        <v>205</v>
+      </c>
+      <c r="F26" s="228"/>
       <c r="G26" s="172"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" thickBot="1">
@@ -11658,20 +11671,32 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="199" t="s">
+      <c r="C30" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="200"/>
-      <c r="E30" s="199" t="s">
+      <c r="D30" s="211"/>
+      <c r="E30" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="201"/>
+      <c r="F30" s="224"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -11684,18 +11709,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11732,103 +11745,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="220" t="s">
+      <c r="C2" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="226"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="220" t="s">
+      <c r="F2" s="200" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="221"/>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:11" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="227"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="224" t="s">
+      <c r="F3" s="202" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="225"/>
+      <c r="G3" s="207"/>
     </row>
     <row r="4" spans="1:11" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="224" t="s">
+      <c r="C4" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="227"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="G4" s="225"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:11" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="224" t="s">
+      <c r="C5" s="202" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="227"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="225"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="207"/>
     </row>
     <row r="6" spans="1:11" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="202" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="227"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="225"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="207"/>
     </row>
     <row r="7" spans="1:11" ht="14.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="214"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="228"/>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="213"/>
+      <c r="B8" s="235"/>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="217"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="214"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="212"/>
-      <c r="F9" s="212"/>
-      <c r="G9" s="213"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" thickBot="1">
-      <c r="B10" s="215"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -12050,10 +12063,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="206" t="s">
+      <c r="C24" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="207"/>
+      <c r="D24" s="209"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -12071,10 +12084,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="218" t="s">
+      <c r="C25" s="222" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="219"/>
+      <c r="D25" s="223"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -12088,10 +12101,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="241" t="s">
+      <c r="C26" s="242" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="242"/>
+      <c r="D26" s="243"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -12110,14 +12123,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="199" t="s">
+      <c r="C29" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="200"/>
-      <c r="E29" s="199" t="s">
+      <c r="D29" s="211"/>
+      <c r="E29" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="201"/>
+      <c r="F29" s="224"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -12134,14 +12147,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="199" t="s">
+      <c r="C32" s="210" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="200"/>
-      <c r="E32" s="199" t="s">
+      <c r="D32" s="211"/>
+      <c r="E32" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="201"/>
+      <c r="F32" s="224"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -12151,20 +12164,29 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="239" t="s">
+      <c r="C33" s="240" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="240"/>
-      <c r="E33" s="241" t="s">
+      <c r="D33" s="241"/>
+      <c r="E33" s="242" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="242"/>
+      <c r="F33" s="243"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -12177,15 +12199,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify Design Data, spec and Detail design.
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_Ver1.1_ANH_THANG_LE.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_Ver1.1_ANH_THANG_LE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER_MLD1\Google Drive\Git Mulodo\System Design - 20902 - API Detail Design\miniblog-le.thang\doc\backend\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER_MLD1\Google Drive\Git Mulodo\Coding 21936 Create User Account\miniblog-le.thang\doc\backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7140" tabRatio="818" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7140" tabRatio="818" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="244">
   <si>
     <t>No</t>
   </si>
@@ -432,13 +432,7 @@
     <t>vutm</t>
   </si>
   <si>
-    <t>b29f1055992addafd37270e601b5ff44</t>
-  </si>
-  <si>
     <t>boitv</t>
-  </si>
-  <si>
-    <t>d9e9c530659814acd65c284e1895b384</t>
   </si>
   <si>
     <t>id</t>
@@ -639,9 +633,6 @@
     <t>11000</t>
   </si>
   <si>
-    <t>0:off, 1: on [create,update,delete,view admin, edit admin]</t>
-  </si>
-  <si>
     <t>Just allow [a-z0-9]</t>
   </si>
   <si>
@@ -809,12 +800,6 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>b29f1055992addafd37270e601b5ff45</t>
-  </si>
-  <si>
-    <t>d9e9c530659814acd65c284e1895b385</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -834,6 +819,24 @@
   </si>
   <si>
     <t>Title post</t>
+  </si>
+  <si>
+    <t>le anh thang</t>
+  </si>
+  <si>
+    <t>nguyen huyen</t>
+  </si>
+  <si>
+    <t>tran vu</t>
+  </si>
+  <si>
+    <t>image1.jpg</t>
+  </si>
+  <si>
+    <t>image2.jpg</t>
+  </si>
+  <si>
+    <t>0:off, 1: on [view,create,update,delete, edit admin]</t>
   </si>
 </sst>
 </file>
@@ -3410,7 +3413,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3957,6 +3960,9 @@
     <xf numFmtId="22" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3967,16 +3973,70 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3988,71 +4048,20 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4071,9 +4080,6 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5807,29 +5813,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="196"/>
-      <c r="P13" s="196"/>
-      <c r="Q13" s="196"/>
-      <c r="R13" s="196"/>
-      <c r="S13" s="196"/>
-      <c r="T13" s="196"/>
-      <c r="U13" s="196"/>
-      <c r="V13" s="196"/>
-      <c r="W13" s="196"/>
-      <c r="X13" s="196"/>
-      <c r="Y13" s="196"/>
-      <c r="Z13" s="196"/>
-      <c r="AA13" s="196"/>
-      <c r="AB13" s="196"/>
-      <c r="AC13" s="196"/>
-      <c r="AD13" s="196"/>
-      <c r="AE13" s="196"/>
-      <c r="AF13" s="196"/>
-      <c r="AG13" s="196"/>
-      <c r="AH13" s="196"/>
-      <c r="AI13" s="196"/>
-      <c r="AJ13" s="196"/>
-      <c r="AK13" s="196"/>
+      <c r="O13" s="197"/>
+      <c r="P13" s="197"/>
+      <c r="Q13" s="197"/>
+      <c r="R13" s="197"/>
+      <c r="S13" s="197"/>
+      <c r="T13" s="197"/>
+      <c r="U13" s="197"/>
+      <c r="V13" s="197"/>
+      <c r="W13" s="197"/>
+      <c r="X13" s="197"/>
+      <c r="Y13" s="197"/>
+      <c r="Z13" s="197"/>
+      <c r="AA13" s="197"/>
+      <c r="AB13" s="197"/>
+      <c r="AC13" s="197"/>
+      <c r="AD13" s="197"/>
+      <c r="AE13" s="197"/>
+      <c r="AF13" s="197"/>
+      <c r="AG13" s="197"/>
+      <c r="AH13" s="197"/>
+      <c r="AI13" s="197"/>
+      <c r="AJ13" s="197"/>
+      <c r="AK13" s="197"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5861,29 +5867,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="196"/>
-      <c r="P14" s="196"/>
-      <c r="Q14" s="196"/>
-      <c r="R14" s="196"/>
-      <c r="S14" s="196"/>
-      <c r="T14" s="196"/>
-      <c r="U14" s="196"/>
-      <c r="V14" s="196"/>
-      <c r="W14" s="196"/>
-      <c r="X14" s="196"/>
-      <c r="Y14" s="196"/>
-      <c r="Z14" s="196"/>
-      <c r="AA14" s="196"/>
-      <c r="AB14" s="196"/>
-      <c r="AC14" s="196"/>
-      <c r="AD14" s="196"/>
-      <c r="AE14" s="196"/>
-      <c r="AF14" s="196"/>
-      <c r="AG14" s="196"/>
-      <c r="AH14" s="196"/>
-      <c r="AI14" s="196"/>
-      <c r="AJ14" s="196"/>
-      <c r="AK14" s="196"/>
+      <c r="O14" s="197"/>
+      <c r="P14" s="197"/>
+      <c r="Q14" s="197"/>
+      <c r="R14" s="197"/>
+      <c r="S14" s="197"/>
+      <c r="T14" s="197"/>
+      <c r="U14" s="197"/>
+      <c r="V14" s="197"/>
+      <c r="W14" s="197"/>
+      <c r="X14" s="197"/>
+      <c r="Y14" s="197"/>
+      <c r="Z14" s="197"/>
+      <c r="AA14" s="197"/>
+      <c r="AB14" s="197"/>
+      <c r="AC14" s="197"/>
+      <c r="AD14" s="197"/>
+      <c r="AE14" s="197"/>
+      <c r="AF14" s="197"/>
+      <c r="AG14" s="197"/>
+      <c r="AH14" s="197"/>
+      <c r="AI14" s="197"/>
+      <c r="AJ14" s="197"/>
+      <c r="AK14" s="197"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5911,43 +5917,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="197" t="s">
-        <v>118</v>
-      </c>
-      <c r="L15" s="197"/>
-      <c r="M15" s="197"/>
-      <c r="N15" s="197"/>
-      <c r="O15" s="197"/>
-      <c r="P15" s="197"/>
-      <c r="Q15" s="197"/>
-      <c r="R15" s="197"/>
-      <c r="S15" s="197"/>
-      <c r="T15" s="197"/>
-      <c r="U15" s="197"/>
-      <c r="V15" s="197"/>
-      <c r="W15" s="197"/>
-      <c r="X15" s="197"/>
-      <c r="Y15" s="197"/>
-      <c r="Z15" s="197"/>
-      <c r="AA15" s="197"/>
-      <c r="AB15" s="197"/>
-      <c r="AC15" s="197"/>
-      <c r="AD15" s="197"/>
-      <c r="AE15" s="197"/>
-      <c r="AF15" s="197"/>
-      <c r="AG15" s="197"/>
-      <c r="AH15" s="197"/>
-      <c r="AI15" s="197"/>
-      <c r="AJ15" s="197"/>
-      <c r="AK15" s="197"/>
-      <c r="AL15" s="197"/>
-      <c r="AM15" s="197"/>
-      <c r="AN15" s="197"/>
-      <c r="AO15" s="197"/>
-      <c r="AP15" s="197"/>
-      <c r="AQ15" s="197"/>
-      <c r="AR15" s="197"/>
-      <c r="AS15" s="197"/>
+      <c r="K15" s="198" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="198"/>
+      <c r="M15" s="198"/>
+      <c r="N15" s="198"/>
+      <c r="O15" s="198"/>
+      <c r="P15" s="198"/>
+      <c r="Q15" s="198"/>
+      <c r="R15" s="198"/>
+      <c r="S15" s="198"/>
+      <c r="T15" s="198"/>
+      <c r="U15" s="198"/>
+      <c r="V15" s="198"/>
+      <c r="W15" s="198"/>
+      <c r="X15" s="198"/>
+      <c r="Y15" s="198"/>
+      <c r="Z15" s="198"/>
+      <c r="AA15" s="198"/>
+      <c r="AB15" s="198"/>
+      <c r="AC15" s="198"/>
+      <c r="AD15" s="198"/>
+      <c r="AE15" s="198"/>
+      <c r="AF15" s="198"/>
+      <c r="AG15" s="198"/>
+      <c r="AH15" s="198"/>
+      <c r="AI15" s="198"/>
+      <c r="AJ15" s="198"/>
+      <c r="AK15" s="198"/>
+      <c r="AL15" s="198"/>
+      <c r="AM15" s="198"/>
+      <c r="AN15" s="198"/>
+      <c r="AO15" s="198"/>
+      <c r="AP15" s="198"/>
+      <c r="AQ15" s="198"/>
+      <c r="AR15" s="198"/>
+      <c r="AS15" s="198"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5967,41 +5973,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="197"/>
-      <c r="L16" s="197"/>
-      <c r="M16" s="197"/>
-      <c r="N16" s="197"/>
-      <c r="O16" s="197"/>
-      <c r="P16" s="197"/>
-      <c r="Q16" s="197"/>
-      <c r="R16" s="197"/>
-      <c r="S16" s="197"/>
-      <c r="T16" s="197"/>
-      <c r="U16" s="197"/>
-      <c r="V16" s="197"/>
-      <c r="W16" s="197"/>
-      <c r="X16" s="197"/>
-      <c r="Y16" s="197"/>
-      <c r="Z16" s="197"/>
-      <c r="AA16" s="197"/>
-      <c r="AB16" s="197"/>
-      <c r="AC16" s="197"/>
-      <c r="AD16" s="197"/>
-      <c r="AE16" s="197"/>
-      <c r="AF16" s="197"/>
-      <c r="AG16" s="197"/>
-      <c r="AH16" s="197"/>
-      <c r="AI16" s="197"/>
-      <c r="AJ16" s="197"/>
-      <c r="AK16" s="197"/>
-      <c r="AL16" s="197"/>
-      <c r="AM16" s="197"/>
-      <c r="AN16" s="197"/>
-      <c r="AO16" s="197"/>
-      <c r="AP16" s="197"/>
-      <c r="AQ16" s="197"/>
-      <c r="AR16" s="197"/>
-      <c r="AS16" s="197"/>
+      <c r="K16" s="198"/>
+      <c r="L16" s="198"/>
+      <c r="M16" s="198"/>
+      <c r="N16" s="198"/>
+      <c r="O16" s="198"/>
+      <c r="P16" s="198"/>
+      <c r="Q16" s="198"/>
+      <c r="R16" s="198"/>
+      <c r="S16" s="198"/>
+      <c r="T16" s="198"/>
+      <c r="U16" s="198"/>
+      <c r="V16" s="198"/>
+      <c r="W16" s="198"/>
+      <c r="X16" s="198"/>
+      <c r="Y16" s="198"/>
+      <c r="Z16" s="198"/>
+      <c r="AA16" s="198"/>
+      <c r="AB16" s="198"/>
+      <c r="AC16" s="198"/>
+      <c r="AD16" s="198"/>
+      <c r="AE16" s="198"/>
+      <c r="AF16" s="198"/>
+      <c r="AG16" s="198"/>
+      <c r="AH16" s="198"/>
+      <c r="AI16" s="198"/>
+      <c r="AJ16" s="198"/>
+      <c r="AK16" s="198"/>
+      <c r="AL16" s="198"/>
+      <c r="AM16" s="198"/>
+      <c r="AN16" s="198"/>
+      <c r="AO16" s="198"/>
+      <c r="AP16" s="198"/>
+      <c r="AQ16" s="198"/>
+      <c r="AR16" s="198"/>
+      <c r="AS16" s="198"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6590,14 +6596,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="198">
+      <c r="AN27" s="199">
         <v>42310</v>
       </c>
-      <c r="AO27" s="198"/>
-      <c r="AP27" s="198"/>
-      <c r="AQ27" s="198"/>
-      <c r="AR27" s="198"/>
-      <c r="AS27" s="198"/>
+      <c r="AO27" s="199"/>
+      <c r="AP27" s="199"/>
+      <c r="AQ27" s="199"/>
+      <c r="AR27" s="199"/>
+      <c r="AS27" s="199"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7087,105 +7093,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
+      <c r="C2" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="201"/>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
+      <c r="F2" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="204"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="202" t="s">
+      <c r="F3" s="226" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="207"/>
+      <c r="G3" s="227"/>
     </row>
     <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
+      <c r="C4" s="226" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="203"/>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202"/>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
+      <c r="C5" s="226" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="203"/>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
+      <c r="C6" s="226" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="203"/>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:7" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="235" t="s">
+      <c r="B8" s="230" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -7311,10 +7317,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="222" t="s">
+      <c r="C20" s="220" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="223"/>
+      <c r="D20" s="221"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -7328,10 +7334,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="240" t="s">
+      <c r="C21" s="241" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="241"/>
+      <c r="D21" s="242"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -7350,14 +7356,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="210" t="s">
+      <c r="C24" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="211"/>
-      <c r="E24" s="210" t="s">
+      <c r="D24" s="202"/>
+      <c r="E24" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="224"/>
+      <c r="F24" s="203"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -7374,14 +7380,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="210" t="s">
+      <c r="C27" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="211"/>
-      <c r="E27" s="210" t="s">
+      <c r="D27" s="202"/>
+      <c r="E27" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="224"/>
+      <c r="F27" s="203"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -7391,23 +7397,14 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="240"/>
-      <c r="D28" s="241"/>
-      <c r="E28" s="242"/>
-      <c r="F28" s="243"/>
+      <c r="C28" s="241"/>
+      <c r="D28" s="242"/>
+      <c r="E28" s="243"/>
+      <c r="F28" s="244"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -7420,6 +7417,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7467,103 +7473,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
+      <c r="C2" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="201"/>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="246" t="s">
+      <c r="F2" s="247" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="247"/>
+      <c r="G2" s="248"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="248" t="s">
+      <c r="F3" s="249" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="207"/>
+      <c r="G3" s="227"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
+      <c r="C4" s="226" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="203"/>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202"/>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
+      <c r="C5" s="226" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="203"/>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
+      <c r="C6" s="226" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="203"/>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="235"/>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="230"/>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -7806,10 +7812,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="222" t="s">
+      <c r="C22" s="220" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="223"/>
+      <c r="D22" s="221"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -7829,10 +7835,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="227" t="s">
+      <c r="C23" s="206" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="228"/>
+      <c r="D23" s="207"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -7850,10 +7856,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="240" t="s">
+      <c r="C24" s="241" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="241"/>
+      <c r="D24" s="242"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -7892,14 +7898,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="210" t="s">
+      <c r="C27" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="211"/>
-      <c r="E27" s="210" t="s">
+      <c r="D27" s="202"/>
+      <c r="E27" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="224"/>
+      <c r="F27" s="203"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -7936,14 +7942,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="210" t="s">
+      <c r="C30" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="211"/>
-      <c r="E30" s="210" t="s">
+      <c r="D30" s="202"/>
+      <c r="E30" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="224"/>
+      <c r="F30" s="203"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -7959,14 +7965,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="222" t="s">
+      <c r="C31" s="220" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="223"/>
-      <c r="E31" s="227" t="s">
+      <c r="D31" s="221"/>
+      <c r="E31" s="206" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="228"/>
+      <c r="F31" s="207"/>
       <c r="G31" s="53" t="s">
         <v>77</v>
       </c>
@@ -7982,14 +7988,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="244" t="s">
+      <c r="C32" s="245" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="245"/>
-      <c r="E32" s="242" t="s">
+      <c r="D32" s="246"/>
+      <c r="E32" s="243" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="243"/>
+      <c r="F32" s="244"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -8042,6 +8048,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -8058,14 +8072,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8129,7 +8135,7 @@
         <v>102</v>
       </c>
       <c r="D3" s="94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E3" s="95" t="s">
         <v>100</v>
@@ -8139,13 +8145,13 @@
     <row r="4" spans="2:6">
       <c r="B4" s="97"/>
       <c r="C4" s="114" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D4" s="94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="99" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F4" s="100"/>
     </row>
@@ -8390,11 +8396,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" thickBot="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -8415,7 +8421,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="130" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8424,10 +8430,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="123" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -8436,10 +8442,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="123" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8448,10 +8454,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8460,7 +8466,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="123" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C7" s="124"/>
     </row>
@@ -8661,8 +8667,8 @@
   </sheetPr>
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -8678,7 +8684,7 @@
     <col min="11" max="11" width="17.7109375" style="13" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="13" customWidth="1"/>
     <col min="13" max="15" width="12.42578125" style="13" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="26" style="13" customWidth="1"/>
     <col min="17" max="18" width="19.28515625" style="13" customWidth="1"/>
     <col min="19" max="19" width="17" style="13" customWidth="1"/>
     <col min="20" max="20" width="15.42578125" style="13" customWidth="1"/>
@@ -8694,107 +8700,107 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="201"/>
+      <c r="C2" s="222" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="204"/>
+      <c r="F2" s="222" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:21" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="205">
+      <c r="F3" s="224">
         <v>42249</v>
       </c>
-      <c r="G3" s="206"/>
+      <c r="G3" s="225"/>
     </row>
     <row r="4" spans="1:21" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="203"/>
+      <c r="C4" s="226" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:21" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
+      <c r="C5" s="226" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="203"/>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:21" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
+      <c r="C6" s="226" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="203"/>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:21" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:21" ht="12" customHeight="1">
-      <c r="B8" s="215" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="213" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:21" ht="12" customHeight="1">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:21" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8827,40 +8833,40 @@
         <v>31</v>
       </c>
       <c r="I13" s="194" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J13" s="194" t="s">
         <v>106</v>
       </c>
       <c r="K13" s="194" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L13" s="187" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M13" s="187" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N13" s="187" t="s">
+        <v>131</v>
+      </c>
+      <c r="O13" s="187" t="s">
+        <v>134</v>
+      </c>
+      <c r="P13" s="187" t="s">
         <v>133</v>
       </c>
-      <c r="O13" s="187" t="s">
-        <v>136</v>
-      </c>
-      <c r="P13" s="187" t="s">
-        <v>135</v>
-      </c>
       <c r="Q13" s="187" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R13" s="194" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S13" s="194" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T13" s="194" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U13" s="194" t="s">
         <v>6</v>
@@ -8871,13 +8877,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -8894,25 +8900,25 @@
         <v>109</v>
       </c>
       <c r="K14" s="186" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="L14" s="186" t="s">
+        <v>221</v>
+      </c>
+      <c r="M14" s="186" t="s">
+        <v>220</v>
+      </c>
+      <c r="N14" s="186">
+        <v>1</v>
+      </c>
+      <c r="O14" s="186" t="s">
         <v>224</v>
       </c>
-      <c r="M14" s="186" t="s">
-        <v>223</v>
-      </c>
-      <c r="N14" s="186">
-        <v>0</v>
-      </c>
-      <c r="O14" s="186" t="s">
-        <v>227</v>
-      </c>
       <c r="P14" s="191" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q14" s="191" t="s">
-        <v>219</v>
+        <v>225</v>
+      </c>
+      <c r="Q14" s="196" t="s">
+        <v>241</v>
       </c>
       <c r="R14" s="186">
         <v>11000</v>
@@ -8933,7 +8939,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C15" s="65" t="s">
         <v>106</v>
@@ -8946,35 +8952,35 @@
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="186">
         <v>2</v>
       </c>
       <c r="J15" s="186" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="186" t="s">
-        <v>112</v>
+        <v>224</v>
       </c>
       <c r="L15" s="186" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M15" s="186" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N15" s="186">
         <v>1</v>
       </c>
       <c r="O15" s="186" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P15" s="191" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q15" s="191" t="s">
-        <v>219</v>
+        <v>233</v>
+      </c>
+      <c r="Q15" s="196" t="s">
+        <v>242</v>
       </c>
       <c r="R15" s="186">
         <v>11000</v>
@@ -8995,48 +9001,48 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H16" s="87"/>
       <c r="I16" s="186">
         <v>3</v>
       </c>
       <c r="J16" s="186" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="K16" s="186" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="L16" s="186" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M16" s="186" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N16" s="186">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16" s="186" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="P16" s="191" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q16" s="191" t="s">
-        <v>219</v>
+        <v>235</v>
+      </c>
+      <c r="Q16" s="196" t="s">
+        <v>241</v>
       </c>
       <c r="R16" s="186">
         <v>11110</v>
@@ -9057,47 +9063,47 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I17" s="186">
         <v>4</v>
       </c>
       <c r="J17" s="186" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="K17" s="186" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L17" s="186" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M17" s="186" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N17" s="186">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O17" s="186" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="P17" s="191" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q17" s="191" t="s">
-        <v>219</v>
+        <v>234</v>
+      </c>
+      <c r="Q17" s="196" t="s">
+        <v>242</v>
       </c>
       <c r="R17" s="186">
         <v>11111</v>
@@ -9118,20 +9124,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="117" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -9140,20 +9146,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -9162,13 +9168,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
@@ -9177,7 +9183,7 @@
         <v>99</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -9186,22 +9192,22 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D21" s="129" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E21" s="66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F21" s="67" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G21" s="106" t="s">
-        <v>178</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15">
@@ -9210,20 +9216,20 @@
         <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E22" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="67"/>
       <c r="G22" s="106" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H22" s="136"/>
     </row>
@@ -9233,20 +9239,20 @@
         <v>10</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D23" s="129" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E23" s="66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F23" s="67"/>
       <c r="G23" s="106" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -9255,20 +9261,20 @@
         <v>11</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E24" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="67"/>
       <c r="G24" s="106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -9280,17 +9286,17 @@
         <v>41</v>
       </c>
       <c r="C25" s="65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D25" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E25" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="67"/>
       <c r="G25" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -9302,17 +9308,17 @@
         <v>41</v>
       </c>
       <c r="C26" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E26" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="67"/>
       <c r="G26" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="12.75" thickBot="1">
@@ -9327,16 +9333,16 @@
         <v>6</v>
       </c>
       <c r="D27" s="157" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E27" s="155" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F27" s="158" t="s">
         <v>99</v>
       </c>
       <c r="G27" s="156" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -9375,10 +9381,10 @@
       <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="222" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="223"/>
+      <c r="C31" s="220" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="221"/>
       <c r="E31" s="46" t="s">
         <v>3</v>
       </c>
@@ -9392,20 +9398,20 @@
         <v>2</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="227" t="s">
-        <v>151</v>
-      </c>
-      <c r="D32" s="228"/>
+        <v>141</v>
+      </c>
+      <c r="C32" s="206" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="207"/>
       <c r="E32" s="52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
@@ -9413,8 +9419,8 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="225"/>
-      <c r="D33" s="226"/>
+      <c r="C33" s="204"/>
+      <c r="D33" s="205"/>
       <c r="E33" s="58"/>
       <c r="F33" s="58"/>
       <c r="G33" s="55"/>
@@ -9431,14 +9437,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="210" t="s">
+      <c r="C36" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="211"/>
-      <c r="E36" s="210" t="s">
+      <c r="D36" s="202"/>
+      <c r="E36" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="224"/>
+      <c r="F36" s="203"/>
       <c r="G36" s="38" t="s">
         <v>38</v>
       </c>
@@ -9455,51 +9461,47 @@
       <c r="B41" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="210" t="s">
+      <c r="C41" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="211"/>
-      <c r="E41" s="210" t="s">
+      <c r="D41" s="202"/>
+      <c r="E41" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="224"/>
+      <c r="F41" s="203"/>
       <c r="G41" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="P14" r:id="rId1"/>
-    <hyperlink ref="P15" r:id="rId2"/>
-    <hyperlink ref="Q14" r:id="rId3"/>
-    <hyperlink ref="Q15" r:id="rId4"/>
-    <hyperlink ref="Q16" r:id="rId5"/>
-    <hyperlink ref="Q17" r:id="rId6"/>
-    <hyperlink ref="P16" r:id="rId7"/>
-    <hyperlink ref="P17" r:id="rId8"/>
+    <hyperlink ref="P17" r:id="rId1"/>
+    <hyperlink ref="P16" r:id="rId2"/>
+    <hyperlink ref="P15" r:id="rId3"/>
+    <hyperlink ref="P14" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
@@ -9519,7 +9521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B21"/>
     </sheetView>
   </sheetViews>
@@ -9550,108 +9552,108 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="201"/>
+      <c r="C2" s="222" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="204"/>
+      <c r="F2" s="222" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:18" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="205">
+      <c r="F3" s="224">
         <f ca="1" xml:space="preserve"> TODAY()</f>
-        <v>42065</v>
-      </c>
-      <c r="G3" s="206"/>
+        <v>42073</v>
+      </c>
+      <c r="G3" s="225"/>
     </row>
     <row r="4" spans="1:18" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="203"/>
+      <c r="C4" s="226" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:18" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="203"/>
+      <c r="C5" s="226" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:18" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="203"/>
+      <c r="C6" s="226" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:18" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="235" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="230" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:18" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:18" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9692,13 +9694,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -9708,28 +9710,28 @@
         <v>50</v>
       </c>
       <c r="I14" s="186" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J14" s="187" t="s">
+        <v>124</v>
+      </c>
+      <c r="K14" s="187" t="s">
+        <v>127</v>
+      </c>
+      <c r="L14" s="187" t="s">
+        <v>128</v>
+      </c>
+      <c r="M14" s="187" t="s">
+        <v>129</v>
+      </c>
+      <c r="N14" s="187" t="s">
+        <v>230</v>
+      </c>
+      <c r="O14" s="186" t="s">
+        <v>125</v>
+      </c>
+      <c r="P14" s="186" t="s">
         <v>126</v>
-      </c>
-      <c r="K14" s="187" t="s">
-        <v>129</v>
-      </c>
-      <c r="L14" s="187" t="s">
-        <v>130</v>
-      </c>
-      <c r="M14" s="187" t="s">
-        <v>131</v>
-      </c>
-      <c r="N14" s="187" t="s">
-        <v>233</v>
-      </c>
-      <c r="O14" s="186" t="s">
-        <v>127</v>
-      </c>
-      <c r="P14" s="186" t="s">
-        <v>128</v>
       </c>
       <c r="Q14" s="188" t="s">
         <v>6</v>
@@ -9741,13 +9743,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -9760,25 +9762,25 @@
         <v>1</v>
       </c>
       <c r="J15" s="190" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K15" s="190" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L15" s="191" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M15" s="190" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N15" s="186">
         <v>2</v>
       </c>
       <c r="O15" s="189" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P15" s="189" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q15" s="192">
         <v>1</v>
@@ -9790,20 +9792,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O16" s="185"/>
       <c r="P16" s="185"/>
@@ -9814,18 +9816,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E17" s="66"/>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -9834,20 +9836,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E18" s="66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -9856,13 +9858,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
@@ -9879,17 +9881,17 @@
         <v>41</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -9901,17 +9903,17 @@
         <v>42</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" thickBot="1">
@@ -9926,7 +9928,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="132" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E22" s="133" t="s">
         <v>3</v>
@@ -9935,7 +9937,7 @@
         <v>99</v>
       </c>
       <c r="G22" s="134" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -9987,10 +9989,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="222" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="223"/>
+      <c r="C28" s="220" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="221"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -10004,20 +10006,20 @@
         <v>2</v>
       </c>
       <c r="B29" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="206" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="207"/>
+      <c r="E29" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="G29" s="53" t="s">
         <v>143</v>
-      </c>
-      <c r="C29" s="227" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="228"/>
-      <c r="E29" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="G29" s="53" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" thickBot="1">
@@ -10025,8 +10027,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="225"/>
-      <c r="D30" s="226"/>
+      <c r="C30" s="204"/>
+      <c r="D30" s="205"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="28"/>
@@ -10043,14 +10045,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="210" t="s">
+      <c r="C33" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="211"/>
-      <c r="E33" s="210" t="s">
+      <c r="D33" s="202"/>
+      <c r="E33" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="224"/>
+      <c r="F33" s="203"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -10058,16 +10060,16 @@
     <row r="34" spans="1:8">
       <c r="A34" s="145"/>
       <c r="B34" s="146"/>
-      <c r="C34" s="233" t="s">
-        <v>233</v>
-      </c>
-      <c r="D34" s="234"/>
-      <c r="E34" s="233" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34" s="234"/>
+      <c r="C34" s="235" t="s">
+        <v>230</v>
+      </c>
+      <c r="D34" s="236"/>
+      <c r="E34" s="235" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="236"/>
       <c r="G34" s="150" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H34" s="137"/>
     </row>
@@ -10098,14 +10100,14 @@
       <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="210" t="s">
+      <c r="C38" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="211"/>
-      <c r="E38" s="210" t="s">
+      <c r="D38" s="202"/>
+      <c r="E38" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="224"/>
+      <c r="F38" s="203"/>
       <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
@@ -10113,16 +10115,16 @@
     <row r="39" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A39" s="140"/>
       <c r="B39" s="139"/>
-      <c r="C39" s="229" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="230"/>
-      <c r="E39" s="231" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" s="232"/>
+      <c r="C39" s="231" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="232"/>
+      <c r="E39" s="233" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="234"/>
       <c r="G39" s="141" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -10131,6 +10133,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10143,18 +10157,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L15" r:id="rId1"/>
@@ -10198,107 +10200,107 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="201"/>
+      <c r="C2" s="222" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="204"/>
+      <c r="F2" s="222" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:20" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="205">
+      <c r="F3" s="224">
         <v>42045</v>
       </c>
-      <c r="G3" s="206"/>
+      <c r="G3" s="225"/>
     </row>
     <row r="4" spans="1:20" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="203"/>
+      <c r="C4" s="226" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:20" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="203"/>
+      <c r="C5" s="226" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:20" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="203"/>
+      <c r="C6" s="226" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:20" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="B8" s="215" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="213" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:20" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:20" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10331,28 +10333,28 @@
         <v>31</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M13" s="13" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q13" s="128"/>
       <c r="R13" s="128"/>
@@ -10364,10 +10366,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>53</v>
@@ -10384,7 +10386,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K14" s="13">
         <v>1</v>
@@ -10399,10 +10401,10 @@
         <v>0</v>
       </c>
       <c r="O14" s="185" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P14" s="185" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q14" s="127"/>
       <c r="R14" s="127"/>
@@ -10414,13 +10416,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -10434,7 +10436,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K15" s="13">
         <v>2</v>
@@ -10449,10 +10451,10 @@
         <v>1</v>
       </c>
       <c r="O15" s="185" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P15" s="185" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="Q15" s="127"/>
       <c r="R15" s="127"/>
@@ -10464,20 +10466,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -10487,20 +10489,20 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" s="65" t="s">
         <v>181</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>184</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -10509,10 +10511,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D18" s="129" t="s">
         <v>53</v>
@@ -10520,7 +10522,7 @@
       <c r="E18" s="66"/>
       <c r="F18" s="67"/>
       <c r="G18" s="117" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -10532,17 +10534,17 @@
         <v>41</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -10554,17 +10556,17 @@
         <v>42</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" thickBot="1">
@@ -10579,7 +10581,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="132" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="133" t="s">
         <v>3</v>
@@ -10588,7 +10590,7 @@
         <v>99</v>
       </c>
       <c r="G21" s="134" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" thickBot="1">
@@ -10624,10 +10626,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="222" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="223"/>
+      <c r="C25" s="220" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="221"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -10641,8 +10643,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="51"/>
-      <c r="C26" s="227"/>
-      <c r="D26" s="228"/>
+      <c r="C26" s="206"/>
+      <c r="D26" s="207"/>
       <c r="E26" s="52"/>
       <c r="F26" s="52"/>
       <c r="G26" s="53"/>
@@ -10652,8 +10654,8 @@
         <v>3</v>
       </c>
       <c r="B27" s="54"/>
-      <c r="C27" s="225"/>
-      <c r="D27" s="226"/>
+      <c r="C27" s="204"/>
+      <c r="D27" s="205"/>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
       <c r="G27" s="55"/>
@@ -10670,14 +10672,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="210" t="s">
+      <c r="C30" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="211"/>
-      <c r="E30" s="210" t="s">
+      <c r="D30" s="202"/>
+      <c r="E30" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="224"/>
+      <c r="F30" s="203"/>
       <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
@@ -10687,16 +10689,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="138"/>
-      <c r="C31" s="230" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="230"/>
-      <c r="E31" s="230" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="230"/>
+      <c r="C31" s="232" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" s="232"/>
+      <c r="E31" s="232" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="232"/>
       <c r="G31" s="160" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="12.75" thickBot="1">
@@ -10704,16 +10706,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="161"/>
-      <c r="C32" s="236" t="s">
-        <v>231</v>
-      </c>
-      <c r="D32" s="236"/>
-      <c r="E32" s="236" t="s">
-        <v>121</v>
-      </c>
-      <c r="F32" s="236"/>
+      <c r="C32" s="237" t="s">
+        <v>228</v>
+      </c>
+      <c r="D32" s="237"/>
+      <c r="E32" s="237" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="237"/>
       <c r="G32" s="149" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" thickBot="1">
@@ -10728,14 +10730,14 @@
       <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="210" t="s">
+      <c r="C35" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="211"/>
-      <c r="E35" s="210" t="s">
+      <c r="D35" s="202"/>
+      <c r="E35" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="224"/>
+      <c r="F35" s="203"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
@@ -10743,14 +10745,14 @@
     <row r="36" spans="1:7">
       <c r="A36" s="159"/>
       <c r="B36" s="138"/>
-      <c r="C36" s="230" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="230"/>
-      <c r="E36" s="230" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="230"/>
+      <c r="C36" s="232" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="232"/>
+      <c r="E36" s="232" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="232"/>
       <c r="G36" s="160"/>
     </row>
     <row r="37" spans="1:7" ht="12.75" thickBot="1">
@@ -10764,18 +10766,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C35:D35"/>
@@ -10790,6 +10780,18 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10828,107 +10830,107 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="201"/>
+      <c r="C2" s="222" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="204"/>
+      <c r="F2" s="222" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="205">
+      <c r="F3" s="224">
         <v>42279</v>
       </c>
-      <c r="G3" s="206"/>
+      <c r="G3" s="225"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="203"/>
+      <c r="C4" s="226" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="203"/>
+      <c r="C5" s="226" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="203"/>
+      <c r="C6" s="226" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="235" t="s">
-        <v>199</v>
-      </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="230" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:14" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10961,19 +10963,19 @@
         <v>31</v>
       </c>
       <c r="I13" s="194" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J13" s="194" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K13" s="187" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="L13" s="187" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M13" s="187" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N13" s="193" t="s">
         <v>6</v>
@@ -10984,10 +10986,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>72</v>
@@ -11004,16 +11006,16 @@
         <v>1</v>
       </c>
       <c r="J14" s="190" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K14" s="190">
         <v>0</v>
       </c>
       <c r="L14" s="189" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M14" s="189" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N14" s="186">
         <v>1</v>
@@ -11025,13 +11027,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -11045,16 +11047,16 @@
         <v>2</v>
       </c>
       <c r="J15" s="190" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K15" s="186">
         <v>1</v>
       </c>
       <c r="L15" s="189" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M15" s="189" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N15" s="186">
         <v>1</v>
@@ -11065,16 +11067,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D16" s="65" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="107"/>
@@ -11089,17 +11091,17 @@
         <v>41</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -11110,17 +11112,17 @@
         <v>42</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" thickBot="1">
@@ -11134,7 +11136,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="132" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E19" s="133" t="s">
         <v>3</v>
@@ -11143,7 +11145,7 @@
         <v>99</v>
       </c>
       <c r="G19" s="134" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" thickBot="1">
@@ -11179,10 +11181,10 @@
       <c r="B23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="222" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="223"/>
+      <c r="C23" s="220" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="221"/>
       <c r="E23" s="46" t="s">
         <v>3</v>
       </c>
@@ -11196,8 +11198,8 @@
         <v>2</v>
       </c>
       <c r="B24" s="51"/>
-      <c r="C24" s="227"/>
-      <c r="D24" s="228"/>
+      <c r="C24" s="206"/>
+      <c r="D24" s="207"/>
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
       <c r="G24" s="53"/>
@@ -11207,8 +11209,8 @@
         <v>3</v>
       </c>
       <c r="B25" s="54"/>
-      <c r="C25" s="225"/>
-      <c r="D25" s="226"/>
+      <c r="C25" s="204"/>
+      <c r="D25" s="205"/>
       <c r="E25" s="58"/>
       <c r="F25" s="58"/>
       <c r="G25" s="55"/>
@@ -11225,14 +11227,14 @@
       <c r="B28" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="210" t="s">
+      <c r="C28" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="211"/>
-      <c r="E28" s="210" t="s">
+      <c r="D28" s="202"/>
+      <c r="E28" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="224"/>
+      <c r="F28" s="203"/>
       <c r="G28" s="38" t="s">
         <v>38</v>
       </c>
@@ -11249,20 +11251,28 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="210" t="s">
+      <c r="C32" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="211"/>
-      <c r="E32" s="210" t="s">
+      <c r="D32" s="202"/>
+      <c r="E32" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="224"/>
+      <c r="F32" s="203"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -11275,14 +11285,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11320,107 +11322,107 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="201"/>
+      <c r="C2" s="222" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="204"/>
+      <c r="F2" s="222" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:12" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="205">
+      <c r="F3" s="224">
         <v>42279</v>
       </c>
-      <c r="G3" s="206"/>
+      <c r="G3" s="225"/>
     </row>
     <row r="4" spans="1:12" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="203"/>
+      <c r="C4" s="226" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:12" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
-        <v>202</v>
-      </c>
-      <c r="D5" s="203"/>
+      <c r="C5" s="226" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:12" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
-        <v>203</v>
-      </c>
-      <c r="D6" s="203"/>
+      <c r="C6" s="226" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:12" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="235" t="s">
-        <v>200</v>
-      </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="230" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11459,10 +11461,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="177" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C14" s="178" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D14" s="178" t="s">
         <v>72</v>
@@ -11476,10 +11478,10 @@
       </c>
       <c r="H14" s="87"/>
       <c r="I14" s="187" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J14" s="187" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K14" s="136"/>
     </row>
@@ -11488,16 +11490,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="153" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C15" s="68" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F15" s="183"/>
       <c r="G15" s="184"/>
@@ -11557,10 +11559,10 @@
       <c r="B19" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="222" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="223"/>
+      <c r="C19" s="220" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="221"/>
       <c r="E19" s="46" t="s">
         <v>3</v>
       </c>
@@ -11574,8 +11576,8 @@
         <v>2</v>
       </c>
       <c r="B20" s="51"/>
-      <c r="C20" s="227"/>
-      <c r="D20" s="228"/>
+      <c r="C20" s="206"/>
+      <c r="D20" s="207"/>
       <c r="E20" s="52"/>
       <c r="F20" s="52"/>
       <c r="G20" s="53"/>
@@ -11585,8 +11587,8 @@
         <v>3</v>
       </c>
       <c r="B21" s="54"/>
-      <c r="C21" s="225"/>
-      <c r="D21" s="226"/>
+      <c r="C21" s="204"/>
+      <c r="D21" s="205"/>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
       <c r="G21" s="55"/>
@@ -11603,14 +11605,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="210" t="s">
+      <c r="C24" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="211"/>
-      <c r="E24" s="210" t="s">
+      <c r="D24" s="202"/>
+      <c r="E24" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="224"/>
+      <c r="F24" s="203"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -11618,27 +11620,27 @@
     <row r="25" spans="1:10">
       <c r="A25" s="168"/>
       <c r="B25" s="169"/>
-      <c r="C25" s="237" t="s">
-        <v>229</v>
-      </c>
-      <c r="D25" s="238"/>
-      <c r="E25" s="237" t="s">
-        <v>204</v>
-      </c>
-      <c r="F25" s="238"/>
+      <c r="C25" s="238" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="239"/>
+      <c r="E25" s="238" t="s">
+        <v>201</v>
+      </c>
+      <c r="F25" s="239"/>
       <c r="G25" s="167"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="170"/>
       <c r="B26" s="171"/>
-      <c r="C26" s="227" t="s">
-        <v>230</v>
-      </c>
-      <c r="D26" s="239"/>
-      <c r="E26" s="227" t="s">
-        <v>205</v>
-      </c>
-      <c r="F26" s="228"/>
+      <c r="C26" s="206" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="240"/>
+      <c r="E26" s="206" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="207"/>
       <c r="G26" s="172"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" thickBot="1">
@@ -11671,20 +11673,32 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="210" t="s">
+      <c r="C30" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="211"/>
-      <c r="E30" s="210" t="s">
+      <c r="D30" s="202"/>
+      <c r="E30" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="224"/>
+      <c r="F30" s="203"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="C18:D18"/>
@@ -11697,18 +11711,6 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11745,103 +11747,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="200" t="s">
+      <c r="C2" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="201"/>
+      <c r="D2" s="228"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="200" t="s">
+      <c r="F2" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="204"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:11" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="229"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="202" t="s">
+      <c r="F3" s="226" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="207"/>
+      <c r="G3" s="227"/>
     </row>
     <row r="4" spans="1:11" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="202" t="s">
+      <c r="C4" s="226" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="203"/>
+      <c r="D4" s="229"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="202"/>
-      <c r="G4" s="207"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="227"/>
     </row>
     <row r="5" spans="1:11" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="202" t="s">
+      <c r="C5" s="226" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="203"/>
+      <c r="D5" s="229"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="207"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="227"/>
     </row>
     <row r="6" spans="1:11" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="202" t="s">
+      <c r="C6" s="226" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="203"/>
+      <c r="D6" s="229"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="207"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="227"/>
     </row>
     <row r="7" spans="1:11" ht="14.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="214"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="235"/>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="217"/>
+      <c r="B8" s="230"/>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="218"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="217"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="215"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" thickBot="1">
-      <c r="B10" s="219"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="219"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -12084,10 +12086,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="222" t="s">
+      <c r="C25" s="220" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="223"/>
+      <c r="D25" s="221"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -12101,10 +12103,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="242" t="s">
+      <c r="C26" s="243" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="243"/>
+      <c r="D26" s="244"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -12123,14 +12125,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="210" t="s">
+      <c r="C29" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="211"/>
-      <c r="E29" s="210" t="s">
+      <c r="D29" s="202"/>
+      <c r="E29" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="224"/>
+      <c r="F29" s="203"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -12147,14 +12149,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="210" t="s">
+      <c r="C32" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="211"/>
-      <c r="E32" s="210" t="s">
+      <c r="D32" s="202"/>
+      <c r="E32" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="224"/>
+      <c r="F32" s="203"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -12164,29 +12166,20 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="240" t="s">
+      <c r="C33" s="241" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="241"/>
-      <c r="E33" s="242" t="s">
+      <c r="D33" s="242"/>
+      <c r="E33" s="243" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="243"/>
+      <c r="F33" s="244"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -12199,6 +12192,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>